<commit_message>
Correction Test et ajouts
</commit_message>
<xml_diff>
--- a/web/test.xlsx
+++ b/web/test.xlsx
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,88 +967,96 @@
       <c r="B47" t="s">
         <v>56</v>
       </c>
+      <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Tous les tests ajoutés
Optimisation en cours
</commit_message>
<xml_diff>
--- a/web/test.xlsx
+++ b/web/test.xlsx
@@ -310,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +335,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -348,11 +354,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +675,8 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -842,7 +850,8 @@
       <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -851,7 +860,8 @@
       <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -860,7 +870,8 @@
       <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -869,7 +880,8 @@
       <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1015,125 +1027,155 @@
       <c r="B55" t="s">
         <v>64</v>
       </c>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>65</v>
       </c>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>66</v>
       </c>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>67</v>
       </c>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>68</v>
       </c>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>69</v>
       </c>
+      <c r="D60" s="2"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>70</v>
       </c>
+      <c r="D61" s="2"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>71</v>
       </c>
+      <c r="D62" s="2"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>72</v>
       </c>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>80</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>82</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>88</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>